<commit_message>
update targets, organize files
</commit_message>
<xml_diff>
--- a/docs/indicator_metadata_template.xlsx
+++ b/docs/indicator_metadata_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\bsb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6010A0D-62D7-4B63-AC79-C47733C1BDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0255BBFB-36A8-42A8-B138-F091A7F28E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53F95F83-0BDB-41B5-A303-D49C340DE854}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>indicator_name</t>
   </si>
@@ -82,6 +82,126 @@
   </si>
   <si>
     <t>NORTH</t>
+  </si>
+  <si>
+    <t>data/BSB_Shelf_Water_Volume_South.txt</t>
+  </si>
+  <si>
+    <t>BSB_Shelf_Water_Volume_South</t>
+  </si>
+  <si>
+    <t>Shelf water volume (km^3) for the Southern stock subunit. Shelf water volume is a measure of the volume of water inshore of the shelf-slope front, a narrow transition region between masses of cool, low salinity shelf water and warm, high salinity slope water. This in-situ data was derived from CTD data from NEFSC surveys and is maintained by Paula Fratantoni.</t>
+  </si>
+  <si>
+    <t>There has been no winter sampling since 2021, no trend for 2024.</t>
+  </si>
+  <si>
+    <t>Shelf water volume is a proxy for suitable winter habitat; higher shelf water volume indicates less suitable habitat, potentially leading to northern fish migrating into the southern subregion.</t>
+  </si>
+  <si>
+    <t>Fratantoni PS, Holzworth-Davis T, Taylor MH. 2015. Description of oceanographic conditions on the Northeast US Continental Shelf during 2014. US Dept Commer, Northeast Fisheries Science Center. Ref Doc. 15-21; 41 p. Available at: http://www.nefsc.noaa.gov/publications/doi:10.7289/V5SQ8XD2</t>
+  </si>
+  <si>
+    <t>SOUTH</t>
+  </si>
+  <si>
+    <t>Shelf water volume (km^3) for the NoBSB_Shelf_Water_Volume_Northrthern stock subunit. Shelf water volume is a measure of the volume of water inshore of the shelf-slope front, a narrow transition region between masses of cool, low salinity shelf water and warm, high salinity slope water. This in-situ data was derived from CTD data from NEFSC surveys and is maintained by Paula Fratantoni.</t>
+  </si>
+  <si>
+    <t>data/BSB_Shelf_Water_Volume_North.txt</t>
+  </si>
+  <si>
+    <t>BSB_Shelf_Water_Volume_North</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Black sea bass is an important Mid-Atlantic stock with high recreational engagement.</t>
+  </si>
+  <si>
+    <t>Catch generally reflects trip patterns. High regulatory complexity is likely contributing to recreational fishing trends.</t>
+  </si>
+  <si>
+    <t>Recent trip numbers are near an all-time high, but may have decreased from 2023.</t>
+  </si>
+  <si>
+    <t>Total annual recreational black sea bass fishing trips for both North and South subunits. Data from NOAA Fisheries’ Marine Recreational Information Program (MRIP).</t>
+  </si>
+  <si>
+    <t>BSB_mrip_trips</t>
+  </si>
+  <si>
+    <t>data/bsb_rec_trips.txt</t>
+  </si>
+  <si>
+    <t>The recreational black sea bass fishery has a catch-and-release component, and management measures are being implemented to reduce recreational harvest.</t>
+  </si>
+  <si>
+    <t>Recreational landings have decreased from 2023 but remain near the long-term average.</t>
+  </si>
+  <si>
+    <t>Total annual recreational landings of black sea bass for both North and South subunits. Data from NOAA Fisheries’ Marine Recreational Information Program (MRIP)</t>
+  </si>
+  <si>
+    <t>data/bsb_rec_landings.txt</t>
+  </si>
+  <si>
+    <t>BSB_mrip_landings</t>
+  </si>
+  <si>
+    <t>Commercial revenue per vessel has an overall increasing trend, despite decreases in both total landings and average price ($/lb).</t>
+  </si>
+  <si>
+    <t>Black sea bass has high commercial value that continues to increase in 2024 despite fewer active vessels in the fleet.</t>
+  </si>
+  <si>
+    <t>Commercial revenue for black sea bass has increased from 2023 and remains well above the long term average</t>
+  </si>
+  <si>
+    <t>Black sea bass commercial revenue (2024 USD)</t>
+  </si>
+  <si>
+    <t>data/bsb_com_revenue.txt</t>
+  </si>
+  <si>
+    <t>BSB_Commercial_Revenue</t>
+  </si>
+  <si>
+    <t>Black sea bass commercial revenue per vessel (2024 USD)</t>
+  </si>
+  <si>
+    <t>data/bsb_com_revenue_per_vessel.txt</t>
+  </si>
+  <si>
+    <t>BSB_Commercial_Revenue_Per_Vessel</t>
+  </si>
+  <si>
+    <t>The number of active vessels has been decreasing since 2017, which could impact revenue distributions and fleet composition."</t>
+  </si>
+  <si>
+    <t>A decrease in targeted black sea bass trips coincides with decreased catch and landings in 2024.</t>
+  </si>
+  <si>
+    <t>Number of commercial vessels has decreased slightly from 2023 and remains well below the long term average.</t>
+  </si>
+  <si>
+    <t>Number of commercial fishing vessels targeting black sea bass</t>
+  </si>
+  <si>
+    <t>data/bsb_com_vessels.txt'</t>
+  </si>
+  <si>
+    <t>BSB_Commercial_Vessels</t>
+  </si>
+  <si>
+    <t>Winter (Feb-Mar) bottom temperature in the black sea bass South stock region. Hubert's data product is a composite before 1993, and from 1993-2019 it is the same as GLORYS. 2020-2024 data are pulled directly from GLORYS. The GLORYS12V1 product is the CMEMS global ocean eddy-resolving (1/12? horizontal resolution, 50 vertical levels) reanalysis.</t>
+  </si>
+  <si>
+    <t>BSB_Winter_Bottom_Temperature_South</t>
+  </si>
+  <si>
+    <t>data/bsb_winter_bottom_temperature_south.txt</t>
   </si>
 </sst>
 </file>
@@ -433,13 +553,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1AD2D4-9856-4933-BB92-256DD2BBE7F0}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -493,6 +616,199 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>